<commit_message>
Bug: Non-quote sheet name special chars
</commit_message>
<xml_diff>
--- a/assets/functions.xlsx
+++ b/assets/functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/coding/excel/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C90FA5-96B3-F74D-A8B3-10EC7D66C5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222628B4-CE08-F74F-A403-40E9649207E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{473E1066-2865-44AB-87BD-B0A68C4D514D}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add: XNPV; Lex floats
</commit_message>
<xml_diff>
--- a/assets/functions.xlsx
+++ b/assets/functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/coding/excel/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222628B4-CE08-F74F-A403-40E9649207E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B8AE5C-514E-B34F-AA4E-E93458BD8D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{473E1066-2865-44AB-87BD-B0A68C4D514D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>INDEX-MATCH-MATCH</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>OFFSET</t>
+  </si>
+  <si>
+    <t>XNPV</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -578,6 +581,15 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <f>XNPV(0.05, B11:F11, B10:F10)</f>
+        <v>7.6576732866908932</v>
+      </c>
+    </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <f>DATE(2022,1,1)</f>

</xml_diff>

<commit_message>
Add: SUMPRODUCT function (close #49)
</commit_message>
<xml_diff>
--- a/assets/functions.xlsx
+++ b/assets/functions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/coding/excel/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/coding/excel-emulator/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD57F05-D803-544B-9A8D-B6F2E44008F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E32007-3111-FA49-9F48-1E5EC8790869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{473E1066-2865-44AB-87BD-B0A68C4D514D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>INDEX-MATCH-MATCH</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>AVERAGEIFS</t>
+  </si>
+  <si>
+    <t>SUMPRODUCT</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -602,6 +605,15 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <f>SUMPRODUCT(C2:C6,D2:D6)</f>
+        <v>530</v>
+      </c>
+    </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <f>DATE(2022,1,1)</f>

</xml_diff>